<commit_message>
constrain to use AustralianAddress
</commit_message>
<xml_diff>
--- a/StructureDefinition-ARFOrganisation.xlsx
+++ b/StructureDefinition-ARFOrganisation.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-23T15:19:20+10:00</t>
+    <t>2024-05-27T13:31:05+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -702,24 +702,24 @@
     <t>Organization.address</t>
   </si>
   <si>
-    <t xml:space="preserve">Address {Address|http://hl7.org.au/fhir/StructureDefinition/au-address}
+    <t xml:space="preserve">Address {http://hl7.org.au/fhir/StructureDefinition/au-address}
 </t>
   </si>
   <si>
-    <t>An address expressed using postal conventions (as opposed to GPS or other location definition formats)</t>
-  </si>
-  <si>
-    <t>An address for the organization.</t>
-  </si>
-  <si>
-    <t>The address is intended to describe postal addresses for administrative purposes, not to describe absolute geographical coordinates. Postal addresses are often used as proxies for physical locations (also see the Location resource).</t>
+    <t>An address in Australia for use within an Australian healthcare context</t>
+  </si>
+  <si>
+    <t>An Australian address expressed using postal conventions (as opposed to GPS or other location definition formats).</t>
+  </si>
+  <si>
+    <t>Note: address is intended to describe postal addresses for administrative purposes, not to describe absolute geographical coordinates.  Postal addresses are often used as proxies for physical locations (also see the [Location](http://hl7.org/fhir/R4/location.html#) resource).</t>
   </si>
   <si>
     <t>May need to keep track of the organization's addresses for contacting, billing or reporting requirements.</t>
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-org-2:An address of an organization can never be of use 'home' {where(use = 'home').empty()}</t>
+inv-add-0:The address shall at least have text or a line {text.exists() or line.exists()}inv-add-1:If asserting no fixed address, the type shall be 'physical' {extension('http://hl7.org.au/fhir/StructureDefinition/no-fixed-address').exists() implies type='physical'}inv-add-2:If asserting no fixed address, the address text shall begin with 'NO FIXED ADDRESS' {extension('http://hl7.org.au/fhir/StructureDefinition/no-fixed-address').exists() implies text.startsWith('NO FIXED ADDRESS')}org-2:An address of an organization can never be of use 'home' {where(use = 'home').empty()}</t>
   </si>
   <si>
     <t>XAD</t>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>78</v>

</xml_diff>